<commit_message>
made some progress on the ml and explanation with plots
</commit_message>
<xml_diff>
--- a/Boussole/Output/Data/performance.xlsx
+++ b/Boussole/Output/Data/performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\petit\Documents\These\Multispectral-Fluorescence\Boussole\Output\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0FF9544-E564-4F0D-B5C7-8952E4A46415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B997A9C-41C1-4C51-9525-DD95B2427254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1068" yWindow="-108" windowWidth="22080" windowHeight="13176" xr2:uid="{486436D1-AEFF-4526-A807-F09DE555A219}"/>
+    <workbookView xWindow="15528" yWindow="1572" windowWidth="16572" windowHeight="9420" xr2:uid="{486436D1-AEFF-4526-A807-F09DE555A219}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>Mean precision</t>
   </si>
@@ -84,9 +84,6 @@
     <t>51.9_10.5)</t>
   </si>
   <si>
-    <t>78.2_12.5)</t>
-  </si>
-  <si>
     <t>63.7_15.4)</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
     <t>65.5_14.8)</t>
   </si>
   <si>
-    <t>75.9_11.6)</t>
-  </si>
-  <si>
     <t>51.9_10.8)</t>
   </si>
   <si>
@@ -130,6 +124,33 @@
   </si>
   <si>
     <t>74.6_9.8</t>
+  </si>
+  <si>
+    <t>no_532</t>
+  </si>
+  <si>
+    <t>64.5_13.2</t>
+  </si>
+  <si>
+    <t>63.5_12.1</t>
+  </si>
+  <si>
+    <t>78.1_14.2)</t>
+  </si>
+  <si>
+    <t>78.5_14.8)</t>
+  </si>
+  <si>
+    <t>77.7_14.5</t>
+  </si>
+  <si>
+    <t>78.6_13.2</t>
+  </si>
+  <si>
+    <t>72.9_10.1</t>
+  </si>
+  <si>
+    <t>72.8_10.7</t>
   </si>
 </sst>
 </file>
@@ -208,9 +229,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -542,33 +566,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22971D49-9217-47C3-B9FE-8E6F44EC8057}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
@@ -581,63 +605,63 @@
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="3">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="35.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="35.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -645,52 +669,52 @@
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="3">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="3">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="35.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="2">
-        <v>3</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="2">
-        <v>3</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="2">
-        <v>2</v>
+    <row r="11" spans="1:4" ht="35.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="3">
+        <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>23</v>
@@ -698,44 +722,86 @@
     </row>
     <row r="12" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="35.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>2</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="3">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="2">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="35.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="2">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="2">
-        <v>2</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes leading to draft V0
</commit_message>
<xml_diff>
--- a/Boussole/Output/Data/performance.xlsx
+++ b/Boussole/Output/Data/performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\petit\Documents\These\Multispectral-Fluorescence\Boussole\Output\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B997A9C-41C1-4C51-9525-DD95B2427254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6390E9-07BF-4433-8CF1-965F5F483AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15528" yWindow="1572" windowWidth="16572" windowHeight="9420" xr2:uid="{486436D1-AEFF-4526-A807-F09DE555A219}"/>
+    <workbookView xWindow="1068" yWindow="-108" windowWidth="22080" windowHeight="13176" xr2:uid="{486436D1-AEFF-4526-A807-F09DE555A219}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>Mean precision</t>
   </si>
@@ -60,97 +60,91 @@
     <t>only_fluo</t>
   </si>
   <si>
-    <t>73.3_10.9</t>
-  </si>
-  <si>
-    <t>59.9_16.1)</t>
-  </si>
-  <si>
-    <t>50.5_8.9)</t>
-  </si>
-  <si>
-    <t>27.2_12.4)</t>
-  </si>
-  <si>
-    <t>76_7.9)</t>
-  </si>
-  <si>
-    <t>63.3_10.7)</t>
-  </si>
-  <si>
-    <t>55_10.7)</t>
-  </si>
-  <si>
-    <t>51.9_10.5)</t>
-  </si>
-  <si>
-    <t>63.7_15.4)</t>
-  </si>
-  <si>
-    <t>69_13.1)</t>
-  </si>
-  <si>
-    <t>47.4_13.2)</t>
-  </si>
-  <si>
-    <t>47.2_13.9)</t>
-  </si>
-  <si>
-    <t>70_12.9)</t>
-  </si>
-  <si>
-    <t>65.5_14.8)</t>
-  </si>
-  <si>
-    <t>51.9_10.8)</t>
-  </si>
-  <si>
-    <t>55.6_10.2)</t>
-  </si>
-  <si>
-    <t>63.7_9.6)</t>
-  </si>
-  <si>
-    <t>77.2_8.2)</t>
-  </si>
-  <si>
-    <t>26.9_11.5)</t>
-  </si>
-  <si>
-    <t>50.8_9.8)</t>
-  </si>
-  <si>
-    <t>59.2_15.4)</t>
-  </si>
-  <si>
-    <t>74.6_9.8</t>
-  </si>
-  <si>
     <t>no_532</t>
   </si>
   <si>
-    <t>64.5_13.2</t>
-  </si>
-  <si>
-    <t>63.5_12.1</t>
-  </si>
-  <si>
-    <t>78.1_14.2)</t>
-  </si>
-  <si>
-    <t>78.5_14.8)</t>
-  </si>
-  <si>
-    <t>77.7_14.5</t>
-  </si>
-  <si>
-    <t>78.6_13.2</t>
-  </si>
-  <si>
-    <t>72.9_10.1</t>
-  </si>
-  <si>
-    <t>72.8_10.7</t>
+    <t>82.3_10.5</t>
+  </si>
+  <si>
+    <t>82.3_9.9</t>
+  </si>
+  <si>
+    <t>77.3_10.8</t>
+  </si>
+  <si>
+    <t>75.3_9.45</t>
+  </si>
+  <si>
+    <t>76.3_10.2</t>
+  </si>
+  <si>
+    <t>76_9.29</t>
+  </si>
+  <si>
+    <t>75_6.9</t>
+  </si>
+  <si>
+    <t>74_7.8</t>
+  </si>
+  <si>
+    <t>75.6_10.4</t>
+  </si>
+  <si>
+    <t>75.3_10.7</t>
+  </si>
+  <si>
+    <t>83.5_10.6</t>
+  </si>
+  <si>
+    <t>84_9.16</t>
+  </si>
+  <si>
+    <t>80.5_12.4</t>
+  </si>
+  <si>
+    <t>79.5_12.4</t>
+  </si>
+  <si>
+    <t>78_10.29</t>
+  </si>
+  <si>
+    <t>76_10.19</t>
+  </si>
+  <si>
+    <t>68_16.9</t>
+  </si>
+  <si>
+    <t>69.5_17.1</t>
+  </si>
+  <si>
+    <t>75.41_12.2</t>
+  </si>
+  <si>
+    <t>76.53_10.7</t>
+  </si>
+  <si>
+    <t>70.9_16.5</t>
+  </si>
+  <si>
+    <t>71.15_17.35</t>
+  </si>
+  <si>
+    <t>66.998_12.25</t>
+  </si>
+  <si>
+    <t>66.92_12.42</t>
+  </si>
+  <si>
+    <t>58.75_11</t>
+  </si>
+  <si>
+    <t>57.69_12.52</t>
+  </si>
+  <si>
+    <t>63.58_8.9</t>
+  </si>
+  <si>
+    <t>63.462_9.06</t>
   </si>
 </sst>
 </file>
@@ -568,11 +562,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22971D49-9217-47C3-B9FE-8E6F44EC8057}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="24.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
@@ -594,7 +591,7 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="35.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>4</v>
       </c>
@@ -602,27 +599,27 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="35.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:4" ht="35.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -630,10 +627,10 @@
         <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="35.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -644,13 +641,13 @@
         <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="35.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -658,10 +655,10 @@
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -672,10 +669,10 @@
         <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -683,13 +680,13 @@
         <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -703,7 +700,7 @@
         <v>13</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="35.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -714,10 +711,10 @@
         <v>6</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -731,7 +728,7 @@
         <v>15</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -742,10 +739,10 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -753,13 +750,13 @@
         <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -770,10 +767,10 @@
         <v>5</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="35.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -784,10 +781,10 @@
         <v>6</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -798,10 +795,10 @@
         <v>7</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>